<commit_message>
IEnumerable and IQueryable difference
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t xml:space="preserve">List </t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>https://github.com/sstechGitHost/DotNet_Collections.git</t>
+  </si>
+  <si>
+    <t>Ienumerable</t>
+  </si>
+  <si>
+    <t>used to process object collections in memory</t>
+  </si>
+  <si>
+    <t>Iqueryable</t>
+  </si>
+  <si>
+    <t>used to query data sources like LINQ to SQL databases</t>
   </si>
 </sst>
 </file>
@@ -504,7 +516,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -683,6 +695,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I28" s="2"/>
     </row>

</xml_diff>